<commit_message>
add manage user page
</commit_message>
<xml_diff>
--- a/_Docs/รายชื่อ user.xlsx
+++ b/_Docs/รายชื่อ user.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pete Ponlachet\Desktop\pms\_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C109632F-CB76-4A98-9FA4-B529C08804D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76609C3-3A5C-4F9B-A2A6-3127C36AE086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43F1A432-E33B-418E-8136-AEBACC847D7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,550 +25,571 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="186">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Prefix</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>StudentID</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>TelephoneNo</t>
+  </si>
+  <si>
+    <t>AcademicYear</t>
+  </si>
+  <si>
+    <t>UserTypeID</t>
+  </si>
+  <si>
+    <t>แบบฟอร์มเพิ่มผู้ใช้</t>
+  </si>
+  <si>
+    <t>user02</t>
+  </si>
+  <si>
+    <t>นาย</t>
+  </si>
+  <si>
+    <t>กฤษติพงศ์</t>
+  </si>
+  <si>
+    <t>ชัยตัน</t>
+  </si>
   <si>
     <t>59543206001-9</t>
   </si>
   <si>
+    <t>user03</t>
+  </si>
+  <si>
+    <t>กิตติธัช</t>
+  </si>
+  <si>
+    <t>วัฒนานุกร</t>
+  </si>
+  <si>
     <t>59543206002-7</t>
   </si>
   <si>
+    <t>user04</t>
+  </si>
+  <si>
+    <t>ชนชนนท์</t>
+  </si>
+  <si>
+    <t>หาวา</t>
+  </si>
+  <si>
     <t>59543206006-8</t>
   </si>
   <si>
+    <t>user05</t>
+  </si>
+  <si>
+    <t>ชาคริต</t>
+  </si>
+  <si>
+    <t>ใจเย็น</t>
+  </si>
+  <si>
     <t>59543206007-6</t>
   </si>
   <si>
+    <t>user06</t>
+  </si>
+  <si>
+    <t>ณัฐสิษธิ์</t>
+  </si>
+  <si>
+    <t>สุขประเสริฐ</t>
+  </si>
+  <si>
     <t>59543206008-4</t>
   </si>
   <si>
+    <t>user07</t>
+  </si>
+  <si>
+    <t>ดัตวศุทธิ์</t>
+  </si>
+  <si>
+    <t>อินผูก</t>
+  </si>
+  <si>
     <t>59543206009-2</t>
   </si>
   <si>
+    <t>user08</t>
+  </si>
+  <si>
+    <t>ธรรมชาติ</t>
+  </si>
+  <si>
+    <t>สุรินทร์</t>
+  </si>
+  <si>
     <t>59543206012-6</t>
   </si>
   <si>
+    <t>user09</t>
+  </si>
+  <si>
+    <t>ปิยพงศ์</t>
+  </si>
+  <si>
+    <t>สุขทองงาม</t>
+  </si>
+  <si>
     <t>59543206015-9</t>
   </si>
   <si>
+    <t>user10</t>
+  </si>
+  <si>
+    <t>นางสาว</t>
+  </si>
+  <si>
+    <t>พงศ์ลดา</t>
+  </si>
+  <si>
+    <t>จิตติกรกาญจน์</t>
+  </si>
+  <si>
     <t>59543206016-7</t>
   </si>
   <si>
+    <t>user11</t>
+  </si>
+  <si>
+    <t>พลเชษฐ์</t>
+  </si>
+  <si>
+    <t>คำมุง</t>
+  </si>
+  <si>
     <t>59543206017-5</t>
   </si>
   <si>
+    <t>user12</t>
+  </si>
+  <si>
+    <t>ภานุเดช</t>
+  </si>
+  <si>
+    <t>ขันธ์สำราญ</t>
+  </si>
+  <si>
     <t>59543206018-3</t>
   </si>
   <si>
+    <t>user13</t>
+  </si>
+  <si>
+    <t>วิรยุทร</t>
+  </si>
+  <si>
+    <t>บัวเพชร</t>
+  </si>
+  <si>
     <t>59543206019-1</t>
   </si>
   <si>
+    <t>user14</t>
+  </si>
+  <si>
+    <t>ศักดิ์ดากรณ์</t>
+  </si>
+  <si>
+    <t>สุขไกว</t>
+  </si>
+  <si>
     <t>59543206020-9</t>
   </si>
   <si>
+    <t>user15</t>
+  </si>
+  <si>
+    <t>ศุภกิจ</t>
+  </si>
+  <si>
+    <t>คิดหมาย</t>
+  </si>
+  <si>
     <t>59543206021-7</t>
   </si>
   <si>
+    <t>user16</t>
+  </si>
+  <si>
+    <t>อิทธิพันธ์</t>
+  </si>
+  <si>
+    <t>พุทธสันตพงศ์</t>
+  </si>
+  <si>
     <t>59543206023-3</t>
   </si>
   <si>
+    <t>user17</t>
+  </si>
+  <si>
+    <t>เอื้ออังกูล</t>
+  </si>
+  <si>
+    <t>พันธ์วงค์</t>
+  </si>
+  <si>
     <t>59543206024-1</t>
   </si>
   <si>
+    <t>user18</t>
+  </si>
+  <si>
+    <t>กฤติพงศ์</t>
+  </si>
+  <si>
+    <t>วชิรางกุล</t>
+  </si>
+  <si>
     <t>59543206026-6</t>
   </si>
   <si>
+    <t>user19</t>
+  </si>
+  <si>
+    <t>จักรกฤษ</t>
+  </si>
+  <si>
+    <t>ทาอภัย</t>
+  </si>
+  <si>
     <t>59543206028-2</t>
   </si>
   <si>
+    <t>user20</t>
+  </si>
+  <si>
+    <t>จิรวัฒน์</t>
+  </si>
+  <si>
+    <t>สุภาธง</t>
+  </si>
+  <si>
     <t>59543206029-0</t>
   </si>
   <si>
+    <t>user21</t>
+  </si>
+  <si>
+    <t>เจษฎา</t>
+  </si>
+  <si>
+    <t>ปราศรัย</t>
+  </si>
+  <si>
     <t>59543206030-8</t>
   </si>
   <si>
+    <t>user22</t>
+  </si>
+  <si>
+    <t>ชนม์แดน</t>
+  </si>
+  <si>
+    <t>อุตตาลกาญจนา</t>
+  </si>
+  <si>
     <t>59543206031-6</t>
   </si>
   <si>
+    <t>user23</t>
+  </si>
+  <si>
+    <t>ชัชวาล</t>
+  </si>
+  <si>
+    <t>ถาคำ</t>
+  </si>
+  <si>
     <t>59543206032-4</t>
   </si>
   <si>
+    <t>user24</t>
+  </si>
+  <si>
+    <t>ชัยชาญ</t>
+  </si>
+  <si>
+    <t>แต้มคู</t>
+  </si>
+  <si>
     <t>59543206033-2</t>
   </si>
   <si>
+    <t>user25</t>
+  </si>
+  <si>
+    <t>ชำนาญ</t>
+  </si>
+  <si>
     <t>59543206034-0</t>
   </si>
   <si>
+    <t>user26</t>
+  </si>
+  <si>
+    <t>ฐิติยา</t>
+  </si>
+  <si>
+    <t>มะโนวัง</t>
+  </si>
+  <si>
     <t>59543206035-7</t>
   </si>
   <si>
+    <t>user27</t>
+  </si>
+  <si>
+    <t>ณัฐดนัย</t>
+  </si>
+  <si>
+    <t>จิระกังวาน</t>
+  </si>
+  <si>
     <t>59543206037-3</t>
   </si>
   <si>
+    <t>user28</t>
+  </si>
+  <si>
+    <t>ทินวัฒน์</t>
+  </si>
+  <si>
+    <t>มูลซาว</t>
+  </si>
+  <si>
     <t>59543206038-1</t>
   </si>
   <si>
+    <t>user29</t>
+  </si>
+  <si>
+    <t>บุญฤทธิ์</t>
+  </si>
+  <si>
+    <t>ดวงหิรัญภักดี</t>
+  </si>
+  <si>
     <t>59543206040-7</t>
   </si>
   <si>
+    <t>user30</t>
+  </si>
+  <si>
+    <t>พงสกร</t>
+  </si>
+  <si>
+    <t>พิทักษ์คณิคกุล</t>
+  </si>
+  <si>
     <t>59543206042-3</t>
   </si>
   <si>
+    <t>user31</t>
+  </si>
+  <si>
+    <t>พฤทธ์บดินทร์</t>
+  </si>
+  <si>
+    <t>ปุณณะบุตร</t>
+  </si>
+  <si>
     <t>59543206043-1</t>
   </si>
   <si>
+    <t>user32</t>
+  </si>
+  <si>
+    <t>พิชญะ</t>
+  </si>
+  <si>
+    <t>อิทร์บัว</t>
+  </si>
+  <si>
     <t>59543206044-9</t>
   </si>
   <si>
+    <t>user33</t>
+  </si>
+  <si>
+    <t>พิสิทธิ์</t>
+  </si>
+  <si>
+    <t>มูลเฟย</t>
+  </si>
+  <si>
     <t>59543206045-6</t>
   </si>
   <si>
+    <t>user34</t>
+  </si>
+  <si>
+    <t>ภาณุวัฒ</t>
+  </si>
+  <si>
+    <t>สืบมงคลชัย</t>
+  </si>
+  <si>
     <t>59543206046-4</t>
   </si>
   <si>
+    <t>user35</t>
+  </si>
+  <si>
+    <t>ภานุพงษ์</t>
+  </si>
+  <si>
+    <t>เทพเมือง</t>
+  </si>
+  <si>
     <t>59543206047-2</t>
   </si>
   <si>
+    <t>user36</t>
+  </si>
+  <si>
+    <t>โรบิ้น</t>
+  </si>
+  <si>
+    <t>ซิ้งค์</t>
+  </si>
+  <si>
     <t>59543206048-0</t>
   </si>
   <si>
+    <t>user37</t>
+  </si>
+  <si>
+    <t>วรภพ</t>
+  </si>
+  <si>
+    <t>โสมนัส</t>
+  </si>
+  <si>
     <t>59543206049-8</t>
   </si>
   <si>
+    <t>user38</t>
+  </si>
+  <si>
+    <t>วุฒิพงษ์</t>
+  </si>
+  <si>
+    <t>สูตรเลข</t>
+  </si>
+  <si>
     <t>59543206052-2</t>
   </si>
   <si>
+    <t>user39</t>
+  </si>
+  <si>
+    <t>สมภพ</t>
+  </si>
+  <si>
+    <t>แก้วขวัญไกร</t>
+  </si>
+  <si>
     <t>59543206054-8</t>
   </si>
   <si>
+    <t>user40</t>
+  </si>
+  <si>
+    <t>สรนันท์</t>
+  </si>
+  <si>
+    <t>จันทาชา</t>
+  </si>
+  <si>
     <t>59543206055-5</t>
   </si>
   <si>
+    <t>user41</t>
+  </si>
+  <si>
+    <t>สุคนธ์ทิพย์</t>
+  </si>
+  <si>
+    <t>โกฏิคำ</t>
+  </si>
+  <si>
     <t>59543206056-3</t>
   </si>
   <si>
+    <t>user42</t>
+  </si>
+  <si>
+    <t>สุทธิรักษา</t>
+  </si>
+  <si>
+    <t>ธรรมใจ</t>
+  </si>
+  <si>
     <t>59543206057-1</t>
   </si>
   <si>
+    <t>user43</t>
+  </si>
+  <si>
+    <t>อัมรินทร์</t>
+  </si>
+  <si>
+    <t>อัมรารัมย์</t>
+  </si>
+  <si>
     <t>59543206058-9</t>
   </si>
   <si>
-    <t>นาย</t>
-  </si>
-  <si>
-    <t>นางสาว</t>
-  </si>
-  <si>
-    <t>กฤษติพงศ์</t>
-  </si>
-  <si>
-    <t>ชัยตัน</t>
-  </si>
-  <si>
-    <t>กิตติธัช</t>
-  </si>
-  <si>
-    <t>วัฒนานุกร</t>
-  </si>
-  <si>
-    <t>ชนชนนท์</t>
-  </si>
-  <si>
-    <t>หาวา</t>
-  </si>
-  <si>
-    <t>ชาคริต</t>
-  </si>
-  <si>
-    <t>ใจเย็น</t>
-  </si>
-  <si>
-    <t>ณัฐสิษธิ์</t>
-  </si>
-  <si>
-    <t>สุขประเสริฐ</t>
-  </si>
-  <si>
-    <t>ดัตวศุทธิ์</t>
-  </si>
-  <si>
-    <t>อินผูก</t>
-  </si>
-  <si>
-    <t>ธรรมชาติ</t>
-  </si>
-  <si>
-    <t>สุรินทร์</t>
-  </si>
-  <si>
-    <t>ปิยพงศ์</t>
-  </si>
-  <si>
-    <t>สุขทองงาม</t>
-  </si>
-  <si>
-    <t>พงศ์ลดา</t>
-  </si>
-  <si>
-    <t>จิตติกรกาญจน์</t>
-  </si>
-  <si>
-    <t>พลเชษฐ์</t>
-  </si>
-  <si>
-    <t>คำมุง</t>
-  </si>
-  <si>
-    <t>ภานุเดช</t>
-  </si>
-  <si>
-    <t>ขันธ์สำราญ</t>
-  </si>
-  <si>
-    <t>วิรยุทร</t>
-  </si>
-  <si>
-    <t>บัวเพชร</t>
-  </si>
-  <si>
-    <t>ศักดิ์ดากรณ์</t>
-  </si>
-  <si>
-    <t>สุขไกว</t>
-  </si>
-  <si>
-    <t>ศุภกิจ</t>
-  </si>
-  <si>
-    <t>คิดหมาย</t>
-  </si>
-  <si>
-    <t>อิทธิพันธ์</t>
-  </si>
-  <si>
-    <t>พุทธสันตพงศ์</t>
-  </si>
-  <si>
-    <t>เอื้ออังกูล</t>
-  </si>
-  <si>
-    <t>พันธ์วงค์</t>
-  </si>
-  <si>
-    <t>กฤติพงศ์</t>
-  </si>
-  <si>
-    <t>วชิรางกุล</t>
-  </si>
-  <si>
-    <t>จักรกฤษ</t>
-  </si>
-  <si>
-    <t>ทาอภัย</t>
-  </si>
-  <si>
-    <t>จิรวัฒน์</t>
-  </si>
-  <si>
-    <t>สุภาธง</t>
-  </si>
-  <si>
-    <t>เจษฎา</t>
-  </si>
-  <si>
-    <t>ปราศรัย</t>
-  </si>
-  <si>
-    <t>ชนม์แดน</t>
-  </si>
-  <si>
-    <t>อุตตาลกาญจนา</t>
-  </si>
-  <si>
-    <t>ชัชวาล</t>
-  </si>
-  <si>
-    <t>ถาคำ</t>
-  </si>
-  <si>
-    <t>ชัยชาญ</t>
-  </si>
-  <si>
-    <t>แต้มคู</t>
-  </si>
-  <si>
-    <t>ชำนาญ</t>
-  </si>
-  <si>
-    <t>ฐิติยา</t>
-  </si>
-  <si>
-    <t>มะโนวัง</t>
-  </si>
-  <si>
-    <t>ณัฐดนัย</t>
-  </si>
-  <si>
-    <t>จิระกังวาน</t>
-  </si>
-  <si>
-    <t>ทินวัฒน์</t>
-  </si>
-  <si>
-    <t>มูลซาว</t>
-  </si>
-  <si>
-    <t>บุญฤทธิ์</t>
-  </si>
-  <si>
-    <t>ดวงหิรัญภักดี</t>
-  </si>
-  <si>
-    <t>พงสกร</t>
-  </si>
-  <si>
-    <t>พิทักษ์คณิคกุล</t>
-  </si>
-  <si>
-    <t>พฤทธ์บดินทร์</t>
-  </si>
-  <si>
-    <t>ปุณณะบุตร</t>
-  </si>
-  <si>
-    <t>พิชญะ</t>
-  </si>
-  <si>
-    <t>อิทร์บัว</t>
-  </si>
-  <si>
-    <t>พิสิทธิ์</t>
-  </si>
-  <si>
-    <t>มูลเฟย</t>
-  </si>
-  <si>
-    <t>ภาณุวัฒ</t>
-  </si>
-  <si>
-    <t>สืบมงคลชัย</t>
-  </si>
-  <si>
-    <t>ภานุพงษ์</t>
-  </si>
-  <si>
-    <t>เทพเมือง</t>
-  </si>
-  <si>
-    <t>โรบิ้น</t>
-  </si>
-  <si>
-    <t>ซิ้งค์</t>
-  </si>
-  <si>
-    <t>วรภพ</t>
-  </si>
-  <si>
-    <t>โสมนัส</t>
-  </si>
-  <si>
-    <t>วุฒิพงษ์</t>
-  </si>
-  <si>
-    <t>สูตรเลข</t>
-  </si>
-  <si>
-    <t>สมภพ</t>
-  </si>
-  <si>
-    <t>แก้วขวัญไกร</t>
-  </si>
-  <si>
-    <t>สรนันท์</t>
-  </si>
-  <si>
-    <t>จันทาชา</t>
-  </si>
-  <si>
-    <t>สุคนธ์ทิพย์</t>
-  </si>
-  <si>
-    <t>โกฏิคำ</t>
-  </si>
-  <si>
-    <t>สุทธิรักษา</t>
-  </si>
-  <si>
-    <t>ธรรมใจ</t>
-  </si>
-  <si>
-    <t>อัมรินทร์</t>
-  </si>
-  <si>
-    <t>อัมรารัมย์</t>
-  </si>
-  <si>
-    <t>user02</t>
-  </si>
-  <si>
-    <t>user03</t>
-  </si>
-  <si>
-    <t>user04</t>
-  </si>
-  <si>
-    <t>user05</t>
-  </si>
-  <si>
-    <t>user06</t>
-  </si>
-  <si>
-    <t>user07</t>
-  </si>
-  <si>
-    <t>user08</t>
-  </si>
-  <si>
-    <t>user09</t>
-  </si>
-  <si>
-    <t>user10</t>
-  </si>
-  <si>
-    <t>user11</t>
-  </si>
-  <si>
-    <t>user12</t>
-  </si>
-  <si>
-    <t>user13</t>
-  </si>
-  <si>
-    <t>user14</t>
-  </si>
-  <si>
-    <t>user15</t>
-  </si>
-  <si>
-    <t>user16</t>
-  </si>
-  <si>
-    <t>user17</t>
-  </si>
-  <si>
-    <t>user18</t>
-  </si>
-  <si>
-    <t>user19</t>
-  </si>
-  <si>
-    <t>user20</t>
-  </si>
-  <si>
-    <t>user21</t>
-  </si>
-  <si>
-    <t>user22</t>
-  </si>
-  <si>
-    <t>user23</t>
-  </si>
-  <si>
-    <t>user24</t>
-  </si>
-  <si>
-    <t>user25</t>
-  </si>
-  <si>
-    <t>user26</t>
-  </si>
-  <si>
-    <t>user27</t>
-  </si>
-  <si>
-    <t>user28</t>
-  </si>
-  <si>
-    <t>user29</t>
-  </si>
-  <si>
-    <t>user30</t>
-  </si>
-  <si>
-    <t>user31</t>
-  </si>
-  <si>
-    <t>user32</t>
-  </si>
-  <si>
-    <t>user33</t>
-  </si>
-  <si>
-    <t>user34</t>
-  </si>
-  <si>
-    <t>user35</t>
-  </si>
-  <si>
-    <t>user36</t>
-  </si>
-  <si>
-    <t>user37</t>
-  </si>
-  <si>
-    <t>user38</t>
-  </si>
-  <si>
-    <t>user39</t>
-  </si>
-  <si>
-    <t>user40</t>
-  </si>
-  <si>
-    <t>user41</t>
-  </si>
-  <si>
-    <t>user42</t>
-  </si>
-  <si>
-    <t>user43</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Prefix</t>
-  </si>
-  <si>
-    <t>Firstname</t>
-  </si>
-  <si>
-    <t>Lastname</t>
-  </si>
-  <si>
-    <t>StudentID</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>TelephoneNo</t>
-  </si>
-  <si>
-    <t>AcademicYear</t>
-  </si>
-  <si>
-    <t>UserTypeID</t>
+    <t>teacher1</t>
+  </si>
+  <si>
+    <t>ปรัชญ์</t>
+  </si>
+  <si>
+    <t>ปิยะวงศ์วิศาล</t>
+  </si>
+  <si>
+    <t>teacher2</t>
+  </si>
+  <si>
+    <t>อนุชล</t>
+  </si>
+  <si>
+    <t>หอมเสียง</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -584,6 +605,30 @@
       <charset val="222"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -594,12 +639,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -607,15 +651,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -928,100 +994,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7E3D020-42B4-47E1-B1DB-832181290C7A}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" t="s">
+    <row r="1" spans="1:10" ht="27" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I2">
-        <v>2559</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="I3">
         <v>2559</v>
@@ -1032,22 +1079,22 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="I4">
         <v>2559</v>
@@ -1058,22 +1105,22 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="I5">
         <v>2559</v>
@@ -1084,22 +1131,22 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="I6">
         <v>2559</v>
@@ -1110,22 +1157,22 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="I7">
         <v>2559</v>
@@ -1136,22 +1183,22 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="I8">
         <v>2559</v>
@@ -1162,22 +1209,22 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="I9">
         <v>2559</v>
@@ -1188,22 +1235,22 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
         <v>43</v>
-      </c>
-      <c r="D10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
       </c>
       <c r="I10">
         <v>2559</v>
@@ -1214,22 +1261,22 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>136</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="I11">
         <v>2559</v>
@@ -1240,22 +1287,22 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="I12">
         <v>2559</v>
@@ -1266,22 +1313,22 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>138</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="I13">
         <v>2559</v>
@@ -1292,22 +1339,22 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="I14">
         <v>2559</v>
@@ -1318,22 +1365,22 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>140</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>140</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="I15">
         <v>2559</v>
@@ -1344,22 +1391,22 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>141</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>141</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="I16">
         <v>2559</v>
@@ -1370,22 +1417,22 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="I17">
         <v>2559</v>
@@ -1396,22 +1443,22 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>143</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>143</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" t="s">
         <v>76</v>
-      </c>
-      <c r="E18" t="s">
-        <v>77</v>
-      </c>
-      <c r="F18" t="s">
-        <v>16</v>
       </c>
       <c r="I18">
         <v>2559</v>
@@ -1422,13 +1469,13 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>144</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
         <v>78</v>
@@ -1437,7 +1484,7 @@
         <v>79</v>
       </c>
       <c r="F19" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="I19">
         <v>2559</v>
@@ -1448,22 +1495,22 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E20" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F20" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="I20">
         <v>2559</v>
@@ -1474,22 +1521,22 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E21" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F21" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="I21">
         <v>2559</v>
@@ -1500,22 +1547,22 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>147</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>147</v>
+        <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E22" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F22" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="I22">
         <v>2559</v>
@@ -1526,22 +1573,22 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>148</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>148</v>
+        <v>93</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="E23" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="F23" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="I23">
         <v>2559</v>
@@ -1552,22 +1599,22 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>149</v>
+        <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>149</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="E24" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="F24" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
       <c r="I24">
         <v>2559</v>
@@ -1578,22 +1625,22 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>150</v>
+        <v>101</v>
       </c>
       <c r="B25" t="s">
-        <v>150</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="E25" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="F25" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="I25">
         <v>2559</v>
@@ -1604,22 +1651,22 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="B26" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="E26" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="F26" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="I26">
         <v>2559</v>
@@ -1630,22 +1677,22 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>152</v>
+        <v>108</v>
       </c>
       <c r="B27" t="s">
-        <v>152</v>
+        <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D27" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="E27" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="F27" t="s">
-        <v>25</v>
+        <v>111</v>
       </c>
       <c r="I27">
         <v>2559</v>
@@ -1656,22 +1703,22 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>153</v>
+        <v>112</v>
       </c>
       <c r="B28" t="s">
-        <v>153</v>
+        <v>112</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="E28" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="F28" t="s">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="I28">
         <v>2559</v>
@@ -1682,22 +1729,22 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="B29" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="C29" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="E29" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="F29" t="s">
-        <v>27</v>
+        <v>119</v>
       </c>
       <c r="I29">
         <v>2559</v>
@@ -1708,22 +1755,22 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="B30" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="E30" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="F30" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="I30">
         <v>2559</v>
@@ -1734,22 +1781,22 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="B31" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="C31" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="E31" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="F31" t="s">
-        <v>29</v>
+        <v>127</v>
       </c>
       <c r="I31">
         <v>2559</v>
@@ -1760,22 +1807,22 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="B32" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="C32" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="E32" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="F32" t="s">
-        <v>30</v>
+        <v>131</v>
       </c>
       <c r="I32">
         <v>2559</v>
@@ -1786,22 +1833,22 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="B33" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="C33" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="E33" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="F33" t="s">
-        <v>31</v>
+        <v>135</v>
       </c>
       <c r="I33">
         <v>2559</v>
@@ -1812,22 +1859,22 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
       <c r="B34" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
       <c r="C34" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
       <c r="E34" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="F34" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
       <c r="I34">
         <v>2559</v>
@@ -1838,22 +1885,22 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="B35" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="C35" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="E35" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="F35" t="s">
-        <v>33</v>
+        <v>143</v>
       </c>
       <c r="I35">
         <v>2559</v>
@@ -1864,22 +1911,22 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="B36" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="C36" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="E36" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="F36" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
       <c r="I36">
         <v>2559</v>
@@ -1890,22 +1937,22 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B37" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C37" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>113</v>
+        <v>149</v>
       </c>
       <c r="E37" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
       <c r="F37" t="s">
-        <v>35</v>
+        <v>151</v>
       </c>
       <c r="I37">
         <v>2559</v>
@@ -1916,22 +1963,22 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="B38" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C38" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="E38" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="F38" t="s">
-        <v>36</v>
+        <v>155</v>
       </c>
       <c r="I38">
         <v>2559</v>
@@ -1942,22 +1989,22 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B39" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C39" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D39" t="s">
-        <v>117</v>
+        <v>157</v>
       </c>
       <c r="E39" t="s">
-        <v>118</v>
+        <v>158</v>
       </c>
       <c r="F39" t="s">
-        <v>37</v>
+        <v>159</v>
       </c>
       <c r="I39">
         <v>2559</v>
@@ -1968,22 +2015,22 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B40" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C40" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D40" t="s">
-        <v>119</v>
+        <v>161</v>
       </c>
       <c r="E40" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="F40" t="s">
-        <v>38</v>
+        <v>163</v>
       </c>
       <c r="I40">
         <v>2559</v>
@@ -1994,22 +2041,22 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
+        <v>164</v>
+      </c>
+      <c r="B41" t="s">
+        <v>164</v>
+      </c>
+      <c r="C41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
+        <v>165</v>
+      </c>
+      <c r="E41" t="s">
         <v>166</v>
       </c>
-      <c r="B41" t="s">
-        <v>166</v>
-      </c>
-      <c r="C41" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" t="s">
-        <v>121</v>
-      </c>
-      <c r="E41" t="s">
-        <v>122</v>
-      </c>
       <c r="F41" t="s">
-        <v>39</v>
+        <v>167</v>
       </c>
       <c r="I41">
         <v>2559</v>
@@ -2020,22 +2067,22 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B42" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C42" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D42" t="s">
-        <v>123</v>
+        <v>169</v>
       </c>
       <c r="E42" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="F42" t="s">
-        <v>40</v>
+        <v>171</v>
       </c>
       <c r="I42">
         <v>2559</v>
@@ -2046,22 +2093,22 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B43" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C43" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D43" t="s">
-        <v>125</v>
+        <v>173</v>
       </c>
       <c r="E43" t="s">
-        <v>126</v>
+        <v>174</v>
       </c>
       <c r="F43" t="s">
-        <v>41</v>
+        <v>175</v>
       </c>
       <c r="I43">
         <v>2559</v>
@@ -2070,8 +2117,78 @@
         <v>1</v>
       </c>
     </row>
+    <row r="44" spans="1:10">
+      <c r="A44" t="s">
+        <v>176</v>
+      </c>
+      <c r="B44" t="s">
+        <v>176</v>
+      </c>
+      <c r="C44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" t="s">
+        <v>177</v>
+      </c>
+      <c r="E44" t="s">
+        <v>178</v>
+      </c>
+      <c r="F44" t="s">
+        <v>179</v>
+      </c>
+      <c r="I44">
+        <v>2559</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" t="s">
+        <v>180</v>
+      </c>
+      <c r="B45" t="s">
+        <v>180</v>
+      </c>
+      <c r="C45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" t="s">
+        <v>181</v>
+      </c>
+      <c r="E45" t="s">
+        <v>182</v>
+      </c>
+      <c r="J45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" t="s">
+        <v>183</v>
+      </c>
+      <c r="B46" t="s">
+        <v>183</v>
+      </c>
+      <c r="C46" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" t="s">
+        <v>184</v>
+      </c>
+      <c r="E46" t="s">
+        <v>185</v>
+      </c>
+      <c r="J46">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
noti on create project
</commit_message>
<xml_diff>
--- a/_Docs/รายชื่อ user.xlsx
+++ b/_Docs/รายชื่อ user.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pete Ponlachet\Desktop\pms\_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76609C3-3A5C-4F9B-A2A6-3127C36AE086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0030934-9C35-4315-837E-4AA2718914B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43F1A432-E33B-418E-8136-AEBACC847D7E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="186">
   <si>
     <t>Username</t>
   </si>
@@ -997,7 +997,7 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1055,8 +1055,8 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
+      <c r="B3">
+        <v>123456</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -1081,8 +1081,8 @@
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
+      <c r="B4">
+        <v>123456</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -1107,8 +1107,8 @@
       <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
-        <v>20</v>
+      <c r="B5">
+        <v>123456</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1133,8 +1133,8 @@
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
-        <v>24</v>
+      <c r="B6">
+        <v>123456</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -1159,8 +1159,8 @@
       <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
-        <v>28</v>
+      <c r="B7">
+        <v>123456</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -1185,8 +1185,8 @@
       <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
-        <v>32</v>
+      <c r="B8">
+        <v>123456</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -1211,8 +1211,8 @@
       <c r="A9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="s">
-        <v>36</v>
+      <c r="B9">
+        <v>123456</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -1237,8 +1237,8 @@
       <c r="A10" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="s">
-        <v>40</v>
+      <c r="B10">
+        <v>123456</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -1263,8 +1263,8 @@
       <c r="A11" t="s">
         <v>44</v>
       </c>
-      <c r="B11" t="s">
-        <v>44</v>
+      <c r="B11">
+        <v>123456</v>
       </c>
       <c r="C11" t="s">
         <v>45</v>
@@ -1289,8 +1289,8 @@
       <c r="A12" t="s">
         <v>49</v>
       </c>
-      <c r="B12" t="s">
-        <v>49</v>
+      <c r="B12">
+        <v>123456</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1315,8 +1315,8 @@
       <c r="A13" t="s">
         <v>53</v>
       </c>
-      <c r="B13" t="s">
-        <v>53</v>
+      <c r="B13">
+        <v>123456</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -1341,8 +1341,8 @@
       <c r="A14" t="s">
         <v>57</v>
       </c>
-      <c r="B14" t="s">
-        <v>57</v>
+      <c r="B14">
+        <v>123456</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -1367,8 +1367,8 @@
       <c r="A15" t="s">
         <v>61</v>
       </c>
-      <c r="B15" t="s">
-        <v>61</v>
+      <c r="B15">
+        <v>123456</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -1393,8 +1393,8 @@
       <c r="A16" t="s">
         <v>65</v>
       </c>
-      <c r="B16" t="s">
-        <v>65</v>
+      <c r="B16">
+        <v>123456</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -1419,8 +1419,8 @@
       <c r="A17" t="s">
         <v>69</v>
       </c>
-      <c r="B17" t="s">
-        <v>69</v>
+      <c r="B17">
+        <v>123456</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -1445,8 +1445,8 @@
       <c r="A18" t="s">
         <v>73</v>
       </c>
-      <c r="B18" t="s">
-        <v>73</v>
+      <c r="B18">
+        <v>123456</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -1471,8 +1471,8 @@
       <c r="A19" t="s">
         <v>77</v>
       </c>
-      <c r="B19" t="s">
-        <v>77</v>
+      <c r="B19">
+        <v>123456</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
@@ -1497,8 +1497,8 @@
       <c r="A20" t="s">
         <v>81</v>
       </c>
-      <c r="B20" t="s">
-        <v>81</v>
+      <c r="B20">
+        <v>123456</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
@@ -1523,8 +1523,8 @@
       <c r="A21" t="s">
         <v>85</v>
       </c>
-      <c r="B21" t="s">
-        <v>85</v>
+      <c r="B21">
+        <v>123456</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
@@ -1549,8 +1549,8 @@
       <c r="A22" t="s">
         <v>89</v>
       </c>
-      <c r="B22" t="s">
-        <v>89</v>
+      <c r="B22">
+        <v>123456</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
@@ -1575,8 +1575,8 @@
       <c r="A23" t="s">
         <v>93</v>
       </c>
-      <c r="B23" t="s">
-        <v>93</v>
+      <c r="B23">
+        <v>123456</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -1601,8 +1601,8 @@
       <c r="A24" t="s">
         <v>97</v>
       </c>
-      <c r="B24" t="s">
-        <v>97</v>
+      <c r="B24">
+        <v>123456</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -1627,8 +1627,8 @@
       <c r="A25" t="s">
         <v>101</v>
       </c>
-      <c r="B25" t="s">
-        <v>101</v>
+      <c r="B25">
+        <v>123456</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
@@ -1653,8 +1653,8 @@
       <c r="A26" t="s">
         <v>105</v>
       </c>
-      <c r="B26" t="s">
-        <v>105</v>
+      <c r="B26">
+        <v>123456</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
@@ -1679,8 +1679,8 @@
       <c r="A27" t="s">
         <v>108</v>
       </c>
-      <c r="B27" t="s">
-        <v>108</v>
+      <c r="B27">
+        <v>123456</v>
       </c>
       <c r="C27" t="s">
         <v>45</v>
@@ -1705,8 +1705,8 @@
       <c r="A28" t="s">
         <v>112</v>
       </c>
-      <c r="B28" t="s">
-        <v>112</v>
+      <c r="B28">
+        <v>123456</v>
       </c>
       <c r="C28" t="s">
         <v>12</v>
@@ -1731,8 +1731,8 @@
       <c r="A29" t="s">
         <v>116</v>
       </c>
-      <c r="B29" t="s">
-        <v>116</v>
+      <c r="B29">
+        <v>123456</v>
       </c>
       <c r="C29" t="s">
         <v>12</v>
@@ -1757,8 +1757,8 @@
       <c r="A30" t="s">
         <v>120</v>
       </c>
-      <c r="B30" t="s">
-        <v>120</v>
+      <c r="B30">
+        <v>123456</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
@@ -1783,8 +1783,8 @@
       <c r="A31" t="s">
         <v>124</v>
       </c>
-      <c r="B31" t="s">
-        <v>124</v>
+      <c r="B31">
+        <v>123456</v>
       </c>
       <c r="C31" t="s">
         <v>12</v>
@@ -1809,8 +1809,8 @@
       <c r="A32" t="s">
         <v>128</v>
       </c>
-      <c r="B32" t="s">
-        <v>128</v>
+      <c r="B32">
+        <v>123456</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
@@ -1835,8 +1835,8 @@
       <c r="A33" t="s">
         <v>132</v>
       </c>
-      <c r="B33" t="s">
-        <v>132</v>
+      <c r="B33">
+        <v>123456</v>
       </c>
       <c r="C33" t="s">
         <v>12</v>
@@ -1861,8 +1861,8 @@
       <c r="A34" t="s">
         <v>136</v>
       </c>
-      <c r="B34" t="s">
-        <v>136</v>
+      <c r="B34">
+        <v>123456</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
@@ -1887,8 +1887,8 @@
       <c r="A35" t="s">
         <v>140</v>
       </c>
-      <c r="B35" t="s">
-        <v>140</v>
+      <c r="B35">
+        <v>123456</v>
       </c>
       <c r="C35" t="s">
         <v>12</v>
@@ -1913,8 +1913,8 @@
       <c r="A36" t="s">
         <v>144</v>
       </c>
-      <c r="B36" t="s">
-        <v>144</v>
+      <c r="B36">
+        <v>123456</v>
       </c>
       <c r="C36" t="s">
         <v>12</v>
@@ -1939,8 +1939,8 @@
       <c r="A37" t="s">
         <v>148</v>
       </c>
-      <c r="B37" t="s">
-        <v>148</v>
+      <c r="B37">
+        <v>123456</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
@@ -1965,8 +1965,8 @@
       <c r="A38" t="s">
         <v>152</v>
       </c>
-      <c r="B38" t="s">
-        <v>152</v>
+      <c r="B38">
+        <v>123456</v>
       </c>
       <c r="C38" t="s">
         <v>12</v>
@@ -1991,8 +1991,8 @@
       <c r="A39" t="s">
         <v>156</v>
       </c>
-      <c r="B39" t="s">
-        <v>156</v>
+      <c r="B39">
+        <v>123456</v>
       </c>
       <c r="C39" t="s">
         <v>12</v>
@@ -2017,8 +2017,8 @@
       <c r="A40" t="s">
         <v>160</v>
       </c>
-      <c r="B40" t="s">
-        <v>160</v>
+      <c r="B40">
+        <v>123456</v>
       </c>
       <c r="C40" t="s">
         <v>12</v>
@@ -2043,8 +2043,8 @@
       <c r="A41" t="s">
         <v>164</v>
       </c>
-      <c r="B41" t="s">
-        <v>164</v>
+      <c r="B41">
+        <v>123456</v>
       </c>
       <c r="C41" t="s">
         <v>12</v>
@@ -2069,8 +2069,8 @@
       <c r="A42" t="s">
         <v>168</v>
       </c>
-      <c r="B42" t="s">
-        <v>168</v>
+      <c r="B42">
+        <v>123456</v>
       </c>
       <c r="C42" t="s">
         <v>45</v>
@@ -2095,8 +2095,8 @@
       <c r="A43" t="s">
         <v>172</v>
       </c>
-      <c r="B43" t="s">
-        <v>172</v>
+      <c r="B43">
+        <v>123456</v>
       </c>
       <c r="C43" t="s">
         <v>12</v>
@@ -2121,8 +2121,8 @@
       <c r="A44" t="s">
         <v>176</v>
       </c>
-      <c r="B44" t="s">
-        <v>176</v>
+      <c r="B44">
+        <v>123456</v>
       </c>
       <c r="C44" t="s">
         <v>12</v>
@@ -2147,8 +2147,8 @@
       <c r="A45" t="s">
         <v>180</v>
       </c>
-      <c r="B45" t="s">
-        <v>180</v>
+      <c r="B45">
+        <v>123456</v>
       </c>
       <c r="C45" t="s">
         <v>12</v>
@@ -2167,8 +2167,8 @@
       <c r="A46" t="s">
         <v>183</v>
       </c>
-      <c r="B46" t="s">
-        <v>183</v>
+      <c r="B46">
+        <v>123456</v>
       </c>
       <c r="C46" t="s">
         <v>12</v>

</xml_diff>